<commit_message>
Started verity table and added graph state
</commit_message>
<xml_diff>
--- a/Rendu_1/VerityTable.xlsx
+++ b/Rendu_1/VerityTable.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hearc365-my.sharepoint.com/personal/gabriel_dostuni_he-arc_ch/Documents/Documents/HeArc/ISC1b/systemes_numériques/LaboSystemNumeric/Rendu_1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="212" documentId="11_AD4DB114E441178AC67DF403BE13D00A693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{205C8820-4FEC-44F7-B2D6-A4C98CF16458}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,15 +24,87 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>reset_i</t>
+  </si>
+  <si>
+    <t>opcode_i</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>PC_inc_o</t>
+  </si>
+  <si>
+    <t>PC_load_o</t>
+  </si>
+  <si>
+    <t>IR_load_o</t>
+  </si>
+  <si>
+    <t>oper_sel_o</t>
+  </si>
+  <si>
+    <t>oper_load_o</t>
+  </si>
+  <si>
+    <t>Accu_load_o</t>
+  </si>
+  <si>
+    <t>CCR_load_o</t>
+  </si>
+  <si>
+    <t>data_wr_o</t>
+  </si>
+  <si>
+    <t>Outputs</t>
+  </si>
+  <si>
+    <t>CCR_i (0)</t>
+  </si>
+  <si>
+    <t>CCR_i  (1)</t>
+  </si>
+  <si>
+    <t>CCR_i (2)</t>
+  </si>
+  <si>
+    <t>CCR_i (3)</t>
+  </si>
+  <si>
+    <t>sRESET</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +123,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +168,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +436,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="16" width="20.77734375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="30" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="2:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="I2:P2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>